<commit_message>
Added Screen capture scenario .. Pending for Testing
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSources/LoginTest-Backup.xlsx
+++ b/src/main/resources/dataSources/LoginTest-Backup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="44">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -569,7 +572,7 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +762,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -954,7 +957,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>